<commit_message>
"Updated .gitignore, PegawaiImport.php, DatabaseSeeder.php, Template Import.xlsx, and kontak.blade.php files"
</commit_message>
<xml_diff>
--- a/public/assets/Template Import.xlsx
+++ b/public/assets/Template Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatih\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\pengelolaKaryawan\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4D8343-0FCD-439B-A82D-F9719FE22371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E920707-6871-48EA-8631-A9C4A514C4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="2960" windowWidth="19200" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2628" yWindow="1104" windowWidth="23040" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
-    <t>Urutan</t>
-  </si>
-  <si>
     <t>NIK Admedika</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Tanggal Masuk Admedika</t>
   </si>
 </sst>
 </file>
@@ -500,12 +500,12 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,115 +516,115 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>